<commit_message>
Changed function output from a dictionary to a array.
Started adding code to iterate through list and import each CAD Block with  a give offset.
</commit_message>
<xml_diff>
--- a/result checker.xlsx
+++ b/result checker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zjak.theron\Desktop\Zjak\Python\Prop Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43328649-E40D-4D5E-90C5-CFBE7614BABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2DF7C2-807C-42ED-91D3-D943B57DF77A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{572DCE98-BA3A-45C2-BC15-F07EACBB9E8A}"/>
   </bookViews>
@@ -390,14 +390,14 @@
   <dimension ref="F2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="6:8" x14ac:dyDescent="0.25">
       <c r="H2">
-        <v>8745</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="4" spans="6:8" x14ac:dyDescent="0.25">
@@ -405,11 +405,11 @@
         <v>5400</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4">
         <f>F4*G4</f>
-        <v>5400</v>
+        <v>10800</v>
       </c>
     </row>
     <row r="5" spans="6:8" x14ac:dyDescent="0.25">
@@ -417,11 +417,11 @@
         <v>2700</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H10" si="0">F5*G5</f>
-        <v>2700</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="6:8" x14ac:dyDescent="0.25">
@@ -453,11 +453,11 @@
         <v>450</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>450</v>
       </c>
     </row>
     <row r="9" spans="6:8" x14ac:dyDescent="0.25">
@@ -465,11 +465,11 @@
         <v>270</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="6:8" x14ac:dyDescent="0.25">
@@ -477,17 +477,17 @@
         <v>90</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="6:8" x14ac:dyDescent="0.25">
       <c r="H11">
         <f>SUM(H4:H10)</f>
-        <v>8280</v>
+        <v>11520</v>
       </c>
     </row>
     <row r="13" spans="6:8" x14ac:dyDescent="0.25">
@@ -496,7 +496,7 @@
       </c>
       <c r="H13">
         <f>H2-H11</f>
-        <v>465</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>